<commit_message>
all autodesk walls done and cover
</commit_message>
<xml_diff>
--- a/openscad/blinds-refs.xlsx
+++ b/openscad/blinds-refs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>wall1_thick</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>distancefromleft</t>
+  </si>
+  <si>
+    <t>wall3slotd</t>
+  </si>
+  <si>
+    <t>wall3sloth</t>
+  </si>
+  <si>
+    <t>adapterh</t>
+  </si>
+  <si>
+    <t>adapterw</t>
+  </si>
+  <si>
+    <t>wall3slotw</t>
   </si>
 </sst>
 </file>
@@ -437,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -681,6 +696,48 @@
       <c r="B27">
         <f>B4 - 18</f>
         <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <f>B31+2+2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <f>B32+2+2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>